<commit_message>
what next to do(Add limit to question, Store answers selected and completion page)
</commit_message>
<xml_diff>
--- a/generated_questions.xlsx
+++ b/generated_questions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>question: What did the Renaissance bring about?</t>
+          <t>question: What did the renaissance of the 14th to 17th centuries mean?</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -509,10 +509,554 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>question: What kind of culture did the Renaissance bring about?</t>
+          <t>question: What did the renaissance of the 14th to 17th centuries produce?</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>question: What is the process by which plants convert sunlight into energy?</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>question: The Renaissance was marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>question: The Renaissance was marked by renewed interest in classical art and learning?</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>question: What is the process by which plants convert sunlight into energy?</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>question: What was the era of the Renaissance?</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>question: What kind of culture was revived during the Renaissance?</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>question: What is the basic process by which plants convert sunlight into energy?</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>question: What was the result of the Renaissance?</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>question: What did the Renaissance period bring about?</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>question: What is the process by which plants convert sunlight into energy?</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>question: What was the nature of the Renaissance?</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>question: What was the nature of the Renaissance period?</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>question: What is the process by which plants convert sunlight into energy?</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>question: The Renaissance was a period of cultural rebirth in Europe in which century?</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>question: The Renaissance was a period of cultural rebirth in Europe in what way?</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>question: What type of energy does photosynthesis produce?</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>question: What did the Renaissance bring about?</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>question: What type of culture did the Renaissance bring?</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>question: What is the basic process by which plants convert sunlight into energy?</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>question: What type of art was revived during the Renaissance?</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>question: What type of art did the Renaissance bring about?</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>question: What is the basic process of photosynthesis?</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Photosynthesis is the process by which plants convert sunlight into chemical energy, producing glucose and oxygen from carbon dioxide and water.</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>question: What is the basic process by which plants convert sunlight into energy?</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>easy</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>question: What type of art and learning did the Renaissance bring about?</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>The Renaissance was a period of cultural rebirth in Europe from the 14th to 17th centuries, marked by renewed interest in classical art and learning.</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>question: What type of art and learning was renewed during the Renaissance?</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
         <is>
           <t>hard</t>
         </is>

</xml_diff>